<commit_message>
Updated with new file versions 1-7-22
</commit_message>
<xml_diff>
--- a/sm_core/Excel_Files/accounts_missing_info.xlsx
+++ b/sm_core/Excel_Files/accounts_missing_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\backup\portfolio\sm_core\Excel_Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sm-core\sm_core\Excel_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73BCEDDE-5F22-452B-956D-369D6B485184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43591DB7-0F81-4268-B32F-630F3200B488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{12CB7AF7-FAFD-409B-B328-9634F82E91E3}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{12CB7AF7-FAFD-409B-B328-9634F82E91E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -464,7 +464,7 @@
   <dimension ref="A1:U20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD20"/>
+      <selection activeCell="A2" sqref="A2:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>